<commit_message>
Remove Docker Compose and GitHub Actions deployment infrastructure, replacing it with manual AWS EC2 setup documentation and updating package scripts.
</commit_message>
<xml_diff>
--- a/feedback.xlsx
+++ b/feedback.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -502,9 +502,49 @@
         <v>2/12/2026, 4:30:35 PM</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1770957814785</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Alfin Sen Varghese</v>
+      </c>
+      <c r="C6" t="str">
+        <v>alfinsen@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>5</v>
+      </c>
+      <c r="E6" t="str">
+        <v>hello..</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2/13/2026, 10:13:34 AM</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1771848606334</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Alfin</v>
+      </c>
+      <c r="C7" t="str">
+        <v>alfin@123</v>
+      </c>
+      <c r="D7" t="str">
+        <v>5</v>
+      </c>
+      <c r="E7" t="str">
+        <v>good!</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2/23/2026, 5:40:06 PM</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>